<commit_message>
Updates to align files with errata
</commit_message>
<xml_diff>
--- a/Figure 3 - bar charts - Net Impacts on Nutrient Avail Myers.xlsx
+++ b/Figure 3 - bar charts - Net Impacts on Nutrient Avail Myers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcole\Documents\Work\R\Nutrition\output\Final Figure Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSULSER\Dropbox (IFPRI)\Everything\RTI-EPA-CCnutrients\Errata\ForGitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC6A68-3723-4668-A5CA-0FCE47016443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182DE995-3076-45E3-9916-B019D3C9EB36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7800" xr2:uid="{347B7581-7DDC-49E8-9DB3-B468751FD348}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{347B7581-7DDC-49E8-9DB3-B468751FD348}"/>
   </bookViews>
   <sheets>
     <sheet name="Myers Protein" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -424,18 +425,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78F0A35-2AF1-4741-86A4-71995DE92BFE}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -457,7 +458,7 @@
         <v>2.5700975920000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -468,7 +469,7 @@
         <v>2.900069201</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -479,7 +480,7 @@
         <v>3.1021088830000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -490,7 +491,7 @@
         <v>2.905214199</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -501,7 +502,7 @@
         <v>2.6948759679999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -512,7 +513,7 @@
         <v>2.8808856729999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -523,7 +524,7 @@
         <v>2.8795806599999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -534,7 +535,7 @@
         <v>3.548623085</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -545,7 +546,7 @@
         <v>2.6280263100000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -556,7 +557,7 @@
         <v>3.0220363749999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -567,7 +568,7 @@
         <v>3.1612389099999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -578,7 +579,7 @@
         <v>3.0169169710000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -589,7 +590,7 @@
         <v>2.7462547119999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -600,7 +601,7 @@
         <v>2.9867530530000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -611,7 +612,7 @@
         <v>2.9566537080000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -631,18 +632,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AE79B6-A220-4A98-A82F-CC5162048D4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -661,10 +662,10 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.0962727889999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.1079723307368847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -672,10 +673,10 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.75524643899999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75726048028968485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -683,10 +684,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2.239453191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.2398674201356004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -694,10 +695,10 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1.530435803</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.5313125594834747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -705,10 +706,10 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1.4667959589999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.4669833072164438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -716,10 +717,10 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>1.8161030339999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.8163234454472712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -727,10 +728,10 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1.945484301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.9454915339490138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -738,10 +739,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1.8541884470000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.8546414690738435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -749,10 +750,10 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>1.1460308219999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.1460308217080248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -760,10 +761,10 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.79024359899999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.79024359930221244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -771,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>2.306726469</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.3067264693676997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -782,10 +783,10 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>1.5973390919999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.5973390916705275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -793,10 +794,10 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>1.5213951880000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.5213951876555238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -804,10 +805,10 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>1.8887406360000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.888740636167979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -815,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>2.014536842</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0145368415507847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -826,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>1.921136137</v>
+        <v>1.9211361366799611</v>
       </c>
     </row>
   </sheetData>
@@ -842,14 +843,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -871,7 +872,7 @@
         <v>1.191707871</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -882,7 +883,7 @@
         <v>0.99067738000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -893,7 +894,7 @@
         <v>3.8309271200000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -904,7 +905,7 @@
         <v>1.612812559</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -915,7 +916,7 @@
         <v>2.2628056120000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -926,7 +927,7 @@
         <v>3.1597138450000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -937,7 +938,7 @@
         <v>3.3541947090000002</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -948,7 +949,7 @@
         <v>2.7261394710000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -959,7 +960,7 @@
         <v>1.218445319</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -970,7 +971,7 @@
         <v>1.034327394</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -981,7 +982,7 @@
         <v>3.9376309589999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -992,7 +993,7 @@
         <v>1.700969824</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>2.3268152770000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>3.3222761730000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>3.4846111240000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>

</xml_diff>